<commit_message>
[master] Current status 26/01/2021
</commit_message>
<xml_diff>
--- a/support_data/purchase_analysis/summary_row.xlsx
+++ b/support_data/purchase_analysis/summary_row.xlsx
@@ -439,31 +439,31 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2">
-        <v>43969</v>
+        <v>44207</v>
       </c>
       <c r="B2" s="2">
-        <v>43971</v>
+        <v>44216</v>
       </c>
       <c r="C2">
-        <v>68659.80976688999</v>
+        <v>22534.30314723</v>
       </c>
       <c r="D2">
-        <v>47785.18778951999</v>
+        <v>18227.88293334</v>
       </c>
       <c r="E2">
-        <v>18835.08</v>
+        <v>5015.074000000001</v>
       </c>
       <c r="F2">
-        <v>2170.08</v>
+        <v>5015.074000000001</v>
       </c>
       <c r="G2">
-        <v>51694.66810475999</v>
+        <v>19047.28366525</v>
       </c>
       <c r="H2">
-        <v>48689.86886209999</v>
+        <v>25657.87662308999</v>
       </c>
       <c r="I2">
-        <v>0.2470898436760764</v>
+        <v>0.1547427253107065</v>
       </c>
     </row>
   </sheetData>

</xml_diff>